<commit_message>
creation of Job 1st part
</commit_message>
<xml_diff>
--- a/target/test-classes/suites/PostModule.xlsx
+++ b/target/test-classes/suites/PostModule.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="PostByImages" sheetId="3" r:id="rId2"/>
-    <sheet name="Post" sheetId="2" r:id="rId3"/>
+    <sheet name="PostAsCircle" sheetId="4" r:id="rId2"/>
+    <sheet name="PostByImages" sheetId="3" r:id="rId3"/>
+    <sheet name="Post" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>TCID</t>
   </si>
@@ -73,16 +74,89 @@
   </si>
   <si>
     <t>PostByImages</t>
+  </si>
+  <si>
+    <t>PostAsCircle</t>
+  </si>
+  <si>
+    <t>PostDescription</t>
+  </si>
+  <si>
+    <t>PostHashTags1</t>
+  </si>
+  <si>
+    <t>PostHashTags2</t>
+  </si>
+  <si>
+    <t>PostHashTags3</t>
+  </si>
+  <si>
+    <t>PostHashTags4</t>
+  </si>
+  <si>
+    <t>PostHashTags5</t>
+  </si>
+  <si>
+    <t>PostHashTags6</t>
+  </si>
+  <si>
+    <t>CircleTitle</t>
+  </si>
+  <si>
+    <t>As a travel blogger, I promote wildlife tourism on my site, such as this recent guide to tiger safaris.</t>
+  </si>
+  <si>
+    <t>auto1</t>
+  </si>
+  <si>
+    <t>auto2</t>
+  </si>
+  <si>
+    <t>auto3</t>
+  </si>
+  <si>
+    <t>auto4</t>
+  </si>
+  <si>
+    <t>auto5</t>
+  </si>
+  <si>
+    <t>auto6</t>
+  </si>
+  <si>
+    <t>Notification request</t>
+  </si>
+  <si>
+    <t>Africa Geographic Tribe</t>
+  </si>
+  <si>
+    <t>Testing mobile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,17 +179,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,6 +543,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -469,10 +561,191 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.77734375" style="2" customWidth="1"/>
+    <col min="7" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,7 +787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>

</xml_diff>